<commit_message>
added optimal prediction analyst
</commit_message>
<xml_diff>
--- a/EmployeesPreferences.xlsx
+++ b/EmployeesPreferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git repozitories\A.I. Work Schedule Generator\A.I.-Work-Schedule-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D45616-5688-4978-95FB-B5EA187014B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3E26E-F476-4067-ACBB-5F9C185572A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{61FF716B-E068-41CD-A55E-546A81C63610}"/>
   </bookViews>
@@ -482,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE4D2F5-3C15-4190-AA5C-B1BD7363096B}">
-  <dimension ref="D1:W15"/>
+  <dimension ref="D2:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,15 +494,10 @@
     <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
     <row r="2" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
     </row>
     <row r="3" spans="4:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E3" s="5" t="s">
@@ -515,11 +510,11 @@
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
         <v>3</v>
       </c>
@@ -530,11 +525,11 @@
       </c>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
     </row>
     <row r="4" spans="4:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D4" s="2" t="s">
@@ -558,13 +553,13 @@
       <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" t="s">
         <v>8</v>
       </c>
       <c r="N4" t="s">
@@ -585,13 +580,13 @@
       <c r="S4" t="s">
         <v>8</v>
       </c>
-      <c r="T4" t="s">
-        <v>6</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="T4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="W4" s="1" t="s">
@@ -620,13 +615,13 @@
       <c r="J5" s="3">
         <v>0</v>
       </c>
-      <c r="K5" s="6">
-        <v>1</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
         <v>0</v>
       </c>
       <c r="N5" s="3">
@@ -647,13 +642,13 @@
       <c r="S5" s="3">
         <v>0</v>
       </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>1</v>
-      </c>
-      <c r="V5" s="3">
+      <c r="T5" s="6">
+        <v>0</v>
+      </c>
+      <c r="U5" s="6">
+        <v>1</v>
+      </c>
+      <c r="V5" s="6">
         <v>0</v>
       </c>
       <c r="W5" s="4">
@@ -683,13 +678,13 @@
       <c r="J6" s="3">
         <v>0</v>
       </c>
-      <c r="K6" s="6">
-        <v>1</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
         <v>0</v>
       </c>
       <c r="N6" s="3">
@@ -710,13 +705,13 @@
       <c r="S6" s="3">
         <v>0</v>
       </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>1</v>
-      </c>
-      <c r="V6" s="3">
+      <c r="T6" s="6">
+        <v>0</v>
+      </c>
+      <c r="U6" s="6">
+        <v>1</v>
+      </c>
+      <c r="V6" s="6">
         <v>0</v>
       </c>
       <c r="W6" s="4">
@@ -746,13 +741,13 @@
       <c r="J7" s="3">
         <v>0</v>
       </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6">
-        <v>1</v>
-      </c>
-      <c r="M7" s="6">
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
         <v>0</v>
       </c>
       <c r="N7" s="3">
@@ -773,13 +768,13 @@
       <c r="S7" s="3">
         <v>0</v>
       </c>
-      <c r="T7" s="3">
-        <v>0</v>
-      </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
+      <c r="T7" s="6">
+        <v>0</v>
+      </c>
+      <c r="U7" s="6">
+        <v>0</v>
+      </c>
+      <c r="V7" s="6">
         <v>1</v>
       </c>
       <c r="W7" s="4">
@@ -809,13 +804,13 @@
       <c r="J8" s="3">
         <v>0</v>
       </c>
-      <c r="K8" s="6">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6">
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
         <v>0</v>
       </c>
       <c r="N8" s="3">
@@ -836,13 +831,13 @@
       <c r="S8" s="3">
         <v>0</v>
       </c>
-      <c r="T8" s="3">
-        <v>0</v>
-      </c>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3">
+      <c r="T8" s="6">
+        <v>0</v>
+      </c>
+      <c r="U8" s="6">
+        <v>0</v>
+      </c>
+      <c r="V8" s="6">
         <v>1</v>
       </c>
       <c r="W8" s="4">
@@ -872,13 +867,13 @@
       <c r="J9" s="3">
         <v>0</v>
       </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <v>1</v>
-      </c>
-      <c r="M9" s="6">
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
         <v>0</v>
       </c>
       <c r="N9" s="3">
@@ -899,13 +894,13 @@
       <c r="S9" s="3">
         <v>0</v>
       </c>
-      <c r="T9" s="3">
-        <v>0</v>
-      </c>
-      <c r="U9" s="3">
-        <v>1</v>
-      </c>
-      <c r="V9" s="3">
+      <c r="T9" s="6">
+        <v>0</v>
+      </c>
+      <c r="U9" s="6">
+        <v>1</v>
+      </c>
+      <c r="V9" s="6">
         <v>0</v>
       </c>
       <c r="W9" s="4">
@@ -935,13 +930,13 @@
       <c r="J10" s="3">
         <v>0</v>
       </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
         <v>1</v>
       </c>
       <c r="N10" s="3">
@@ -962,13 +957,13 @@
       <c r="S10" s="3">
         <v>1</v>
       </c>
-      <c r="T10" s="3">
-        <v>0</v>
-      </c>
-      <c r="U10" s="3">
-        <v>1</v>
-      </c>
-      <c r="V10" s="3">
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6">
+        <v>1</v>
+      </c>
+      <c r="V10" s="6">
         <v>0</v>
       </c>
       <c r="W10" s="4">
@@ -998,13 +993,13 @@
       <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
         <v>1</v>
       </c>
       <c r="N11" s="3">
@@ -1025,13 +1020,13 @@
       <c r="S11" s="3">
         <v>0</v>
       </c>
-      <c r="T11" s="3">
-        <v>1</v>
-      </c>
-      <c r="U11" s="3">
-        <v>0</v>
-      </c>
-      <c r="V11" s="3">
+      <c r="T11" s="6">
+        <v>1</v>
+      </c>
+      <c r="U11" s="6">
+        <v>0</v>
+      </c>
+      <c r="V11" s="6">
         <v>0</v>
       </c>
       <c r="W11" s="4">
@@ -1061,13 +1056,13 @@
       <c r="J12" s="3">
         <v>1</v>
       </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6">
-        <v>1</v>
-      </c>
-      <c r="M12" s="6">
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
         <v>0</v>
       </c>
       <c r="N12" s="3">
@@ -1088,13 +1083,13 @@
       <c r="S12" s="3">
         <v>1</v>
       </c>
-      <c r="T12" s="3">
-        <v>1</v>
-      </c>
-      <c r="U12" s="3">
-        <v>0</v>
-      </c>
-      <c r="V12" s="3">
+      <c r="T12" s="6">
+        <v>1</v>
+      </c>
+      <c r="U12" s="6">
+        <v>0</v>
+      </c>
+      <c r="V12" s="6">
         <v>0</v>
       </c>
       <c r="W12" s="4">
@@ -1130,15 +1125,15 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1166,28 +1161,23 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="T13" s="4">
+      <c r="T13" s="6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U13" s="4">
+      <c r="U13" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="V13" s="4">
+      <c r="V13" s="6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="D4:W13" xr:uid="{3EE4D2F5-3C15-4190-AA5C-B1BD7363096B}"/>

</xml_diff>